<commit_message>
added legends, but really need to adjust widths
</commit_message>
<xml_diff>
--- a/optima/test7pops.xlsx
+++ b/optima/test7pops.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="19410" windowHeight="10950" tabRatio="901" firstSheet="5" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="19410" windowHeight="10950" tabRatio="901" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
-    <sheet name="Populations &amp; programs" sheetId="2" r:id="rId2"/>
+    <sheet name="Populations" sheetId="2" r:id="rId2"/>
     <sheet name="Population size" sheetId="4" r:id="rId3"/>
     <sheet name="HIV prevalence" sheetId="15" r:id="rId4"/>
     <sheet name="Other epidemiology" sheetId="6" r:id="rId5"/>
@@ -454,11 +454,11 @@
   <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="#,##0_ ;\-#,##0\ "/>
-    <numFmt numFmtId="169" formatCode="0.0%"/>
-    <numFmt numFmtId="170" formatCode="#,##0.000"/>
-    <numFmt numFmtId="172" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="#,##0.000"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -829,17 +829,17 @@
     <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -857,26 +857,20 @@
     <xf numFmtId="10" fontId="0" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="67" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="67" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="67" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -915,6 +909,12 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="67" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="67" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="67" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="168">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1395,29 +1395,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
+      <c r="A2" s="49"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
+      <c r="A3" s="49"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
+      <c r="A4" s="28"/>
     </row>
     <row r="5" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="28" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="28"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="29" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1449,37 +1449,37 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="D2" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="E2" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="F2" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="G2" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="H2" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="I2" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C3" s="4"/>
@@ -1492,7 +1492,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C4" s="4"/>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C5" s="4"/>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C6" s="4"/>
@@ -1535,7 +1535,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C7" s="4"/>
@@ -1548,7 +1548,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C8" s="4">
@@ -1565,7 +1565,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C9" s="4"/>
@@ -1583,37 +1583,37 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="D14" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="E14" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="F14" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="G14" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="H14" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="I14" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C15" s="4"/>
@@ -1626,7 +1626,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C16" s="4">
@@ -1643,7 +1643,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C17" s="4"/>
@@ -1658,7 +1658,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C18" s="4"/>
@@ -1671,7 +1671,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C19" s="4"/>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C20" s="4">
@@ -1701,7 +1701,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C21" s="4"/>
@@ -1719,37 +1719,37 @@
     </row>
     <row r="26" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C26" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="D26" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="E26" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="F26" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="G26" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="H26" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="I26" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C27" s="4"/>
@@ -1762,7 +1762,7 @@
     </row>
     <row r="28" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C28" s="4">
@@ -1777,7 +1777,7 @@
     </row>
     <row r="29" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C29" s="4"/>
@@ -1790,7 +1790,7 @@
     </row>
     <row r="30" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C30" s="4"/>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="31" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C31" s="4"/>
@@ -1816,7 +1816,7 @@
     </row>
     <row r="32" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C32" s="4"/>
@@ -1829,7 +1829,7 @@
     </row>
     <row r="33" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C33" s="4"/>
@@ -1847,37 +1847,37 @@
     </row>
     <row r="38" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C38" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="D38" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="E38" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="F38" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="G38" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="H38" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="I38" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B39" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C39" s="4"/>
@@ -1890,7 +1890,7 @@
     </row>
     <row r="40" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B40" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C40" s="4"/>
@@ -1903,7 +1903,7 @@
     </row>
     <row r="41" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B41" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C41" s="4"/>
@@ -1916,7 +1916,7 @@
     </row>
     <row r="42" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B42" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C42" s="4"/>
@@ -1929,7 +1929,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C43" s="4"/>
@@ -1942,7 +1942,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C44" s="4"/>
@@ -1955,7 +1955,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C45" s="4"/>
@@ -1973,37 +1973,37 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C50" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="D50" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="E50" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="F50" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="G50" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="H50" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="I50" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B51" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C51" s="4"/>
@@ -2018,7 +2018,7 @@
     </row>
     <row r="52" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B52" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C52" s="4"/>
@@ -2033,7 +2033,7 @@
     </row>
     <row r="53" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B53" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C53" s="4"/>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="54" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B54" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C54" s="4"/>
@@ -2059,7 +2059,7 @@
     </row>
     <row r="55" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B55" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C55" s="4"/>
@@ -2072,7 +2072,7 @@
     </row>
     <row r="56" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B56" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C56" s="4"/>
@@ -2085,7 +2085,7 @@
     </row>
     <row r="57" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B57" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C57" s="4"/>
@@ -2110,7 +2110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
@@ -2120,1078 +2120,1078 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="44" t="s">
+      <c r="A2" s="38"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="42" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="43" t="s">
+      <c r="A3" s="38"/>
+      <c r="B3" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="44">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="44">
         <v>1E-4</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="44">
         <v>1.4E-3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="43" t="s">
+      <c r="A4" s="38"/>
+      <c r="B4" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="44">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="44">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="44">
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="43" t="s">
+      <c r="A5" s="38"/>
+      <c r="B5" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="44">
         <v>1.38E-2</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="44">
         <v>1.0200000000000001E-2</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="44">
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="43" t="s">
+      <c r="A6" s="38"/>
+      <c r="B6" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="44">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="44">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="44">
         <v>2.8E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="43" t="s">
+      <c r="A7" s="38"/>
+      <c r="B7" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="44">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="44">
         <v>6.3E-3</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="44">
         <v>2.4E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="43" t="s">
+      <c r="A8" s="38"/>
+      <c r="B8" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="44">
         <v>0.36699999999999999</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="44">
         <v>0.29399999999999998</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="44">
         <v>0.44</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="43" t="s">
+      <c r="A9" s="38"/>
+      <c r="B9" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="44">
         <v>0.20499999999999999</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="44">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="44">
         <v>0.27</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="44" t="s">
+      <c r="A14" s="38"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="42" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
-      <c r="B15" s="43" t="s">
+      <c r="A15" s="38"/>
+      <c r="B15" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="45">
+      <c r="C15" s="43">
         <v>26.03</v>
       </c>
-      <c r="D15" s="45">
+      <c r="D15" s="43">
         <v>2</v>
       </c>
-      <c r="E15" s="45">
+      <c r="E15" s="43">
         <v>48.02</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="43" t="s">
+      <c r="A16" s="38"/>
+      <c r="B16" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="45">
+      <c r="C16" s="43">
         <v>1</v>
       </c>
-      <c r="D16" s="45">
+      <c r="D16" s="43">
         <v>1</v>
       </c>
-      <c r="E16" s="45">
+      <c r="E16" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
-      <c r="B17" s="43" t="s">
+      <c r="A17" s="38"/>
+      <c r="B17" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="45">
+      <c r="C17" s="43">
         <v>1</v>
       </c>
-      <c r="D17" s="45">
+      <c r="D17" s="43">
         <v>1</v>
       </c>
-      <c r="E17" s="45">
+      <c r="E17" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
-      <c r="B18" s="43" t="s">
+      <c r="A18" s="38"/>
+      <c r="B18" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="45">
+      <c r="C18" s="43">
         <v>1</v>
       </c>
-      <c r="D18" s="45">
+      <c r="D18" s="43">
         <v>1</v>
       </c>
-      <c r="E18" s="45">
+      <c r="E18" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
-      <c r="B19" s="43" t="s">
+      <c r="A19" s="38"/>
+      <c r="B19" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="45">
+      <c r="C19" s="43">
         <v>3.49</v>
       </c>
-      <c r="D19" s="45">
+      <c r="D19" s="43">
         <v>1.76</v>
       </c>
-      <c r="E19" s="45">
+      <c r="E19" s="43">
         <v>6.92</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
-      <c r="B20" s="43" t="s">
+      <c r="A20" s="38"/>
+      <c r="B20" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="45">
+      <c r="C20" s="43">
         <v>7.17</v>
       </c>
-      <c r="D20" s="45">
+      <c r="D20" s="43">
         <v>3.9</v>
       </c>
-      <c r="E20" s="45">
+      <c r="E20" s="43">
         <v>12.08</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="40"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="44" t="s">
+      <c r="A25" s="38"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="44" t="s">
+      <c r="D25" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="44" t="s">
+      <c r="E25" s="42" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="40"/>
-      <c r="B26" s="43" t="s">
+      <c r="A26" s="38"/>
+      <c r="B26" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="47">
+      <c r="C26" s="45">
         <v>4.1399999999999997</v>
       </c>
-      <c r="D26" s="47">
+      <c r="D26" s="45">
         <v>2</v>
       </c>
-      <c r="E26" s="47">
+      <c r="E26" s="45">
         <v>9.76</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="40"/>
-      <c r="B27" s="43" t="s">
+      <c r="A27" s="38"/>
+      <c r="B27" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="47">
+      <c r="C27" s="45">
         <v>1.05</v>
       </c>
-      <c r="D27" s="47">
+      <c r="D27" s="45">
         <v>0.86</v>
       </c>
-      <c r="E27" s="47">
+      <c r="E27" s="45">
         <v>1.61</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
-      <c r="B28" s="43" t="s">
+      <c r="A28" s="38"/>
+      <c r="B28" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="47">
+      <c r="C28" s="45">
         <v>0.33</v>
       </c>
-      <c r="D28" s="47">
+      <c r="D28" s="45">
         <v>0.32</v>
       </c>
-      <c r="E28" s="47">
+      <c r="E28" s="45">
         <v>0.35</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="40"/>
-      <c r="B29" s="43" t="s">
+      <c r="A29" s="38"/>
+      <c r="B29" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="47">
+      <c r="C29" s="45">
         <v>0.27</v>
       </c>
-      <c r="D29" s="47">
+      <c r="D29" s="45">
         <v>0.25</v>
       </c>
-      <c r="E29" s="47">
+      <c r="E29" s="45">
         <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="40"/>
-      <c r="B30" s="43" t="s">
+      <c r="A30" s="38"/>
+      <c r="B30" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="C30" s="47">
+      <c r="C30" s="45">
         <v>0.67</v>
       </c>
-      <c r="D30" s="47">
+      <c r="D30" s="45">
         <v>0.44</v>
       </c>
-      <c r="E30" s="47">
+      <c r="E30" s="45">
         <v>0.88</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="40"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
+      <c r="A31" s="38"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="40"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="40"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
+      <c r="A33" s="38"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="41" t="s">
+      <c r="A34" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="B34" s="42"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="40"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="44" t="s">
+      <c r="A35" s="38"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="44" t="s">
+      <c r="D35" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E35" s="44" t="s">
+      <c r="E35" s="42" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="40"/>
-      <c r="B36" s="43" t="s">
+      <c r="A36" s="38"/>
+      <c r="B36" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="47">
+      <c r="C36" s="45">
         <v>0.45</v>
       </c>
-      <c r="D36" s="47">
+      <c r="D36" s="45">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E36" s="47">
+      <c r="E36" s="45">
         <v>0.93</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="40"/>
-      <c r="B37" s="43" t="s">
+      <c r="A37" s="38"/>
+      <c r="B37" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="47">
+      <c r="C37" s="45">
         <v>0.7</v>
       </c>
-      <c r="D37" s="47">
+      <c r="D37" s="45">
         <v>0.28999999999999998</v>
       </c>
-      <c r="E37" s="47">
+      <c r="E37" s="45">
         <v>1.1100000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="40"/>
-      <c r="B38" s="43" t="s">
+      <c r="A38" s="38"/>
+      <c r="B38" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="47">
+      <c r="C38" s="45">
         <v>0.47</v>
       </c>
-      <c r="D38" s="47">
+      <c r="D38" s="45">
         <v>0.33</v>
       </c>
-      <c r="E38" s="47">
+      <c r="E38" s="45">
         <v>0.72</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="40"/>
-      <c r="B39" s="43" t="s">
+      <c r="A39" s="38"/>
+      <c r="B39" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="47">
+      <c r="C39" s="45">
         <v>1.52</v>
       </c>
-      <c r="D39" s="47">
+      <c r="D39" s="45">
         <v>1.06</v>
       </c>
-      <c r="E39" s="47">
+      <c r="E39" s="45">
         <v>1.96</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="40"/>
-      <c r="B40" s="42"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="40"/>
+      <c r="A40" s="38"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="40"/>
-      <c r="B41" s="42"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="40"/>
+      <c r="A41" s="38"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="40"/>
-      <c r="B42" s="42"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
+      <c r="A42" s="38"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="41" t="s">
+      <c r="A43" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="B43" s="42"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="40"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="40"/>
-      <c r="B44" s="42"/>
-      <c r="C44" s="44" t="s">
+      <c r="A44" s="38"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D44" s="44" t="s">
+      <c r="D44" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E44" s="44" t="s">
+      <c r="E44" s="42" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="40"/>
-      <c r="B45" s="43" t="s">
+      <c r="A45" s="38"/>
+      <c r="B45" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="C45" s="48">
+      <c r="C45" s="46">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="D45" s="48">
+      <c r="D45" s="46">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="E45" s="48">
+      <c r="E45" s="46">
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="40"/>
-      <c r="B46" s="43" t="s">
+      <c r="A46" s="38"/>
+      <c r="B46" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C46" s="48">
+      <c r="C46" s="46">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="D46" s="48">
+      <c r="D46" s="46">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="E46" s="48">
+      <c r="E46" s="46">
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="40"/>
-      <c r="B47" s="43" t="s">
+      <c r="A47" s="38"/>
+      <c r="B47" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="C47" s="48">
+      <c r="C47" s="46">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="D47" s="48">
+      <c r="D47" s="46">
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="E47" s="48">
+      <c r="E47" s="46">
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="40"/>
-      <c r="B48" s="43" t="s">
+      <c r="A48" s="38"/>
+      <c r="B48" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C48" s="48">
+      <c r="C48" s="46">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="D48" s="48">
+      <c r="D48" s="46">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="E48" s="48">
+      <c r="E48" s="46">
         <v>1.01E-2</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="40"/>
-      <c r="B49" s="43" t="s">
+      <c r="A49" s="38"/>
+      <c r="B49" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="C49" s="48">
+      <c r="C49" s="46">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="D49" s="48">
+      <c r="D49" s="46">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="E49" s="48">
+      <c r="E49" s="46">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="F49" s="40"/>
-      <c r="G49" s="40"/>
-      <c r="H49" s="40"/>
-      <c r="I49" s="40"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="38"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="38"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="40"/>
-      <c r="B50" s="43" t="s">
+      <c r="A50" s="38"/>
+      <c r="B50" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="C50" s="48">
+      <c r="C50" s="46">
         <v>0.32300000000000001</v>
       </c>
-      <c r="D50" s="48">
+      <c r="D50" s="46">
         <v>0.29599999999999999</v>
       </c>
-      <c r="E50" s="48">
+      <c r="E50" s="46">
         <v>0.432</v>
       </c>
-      <c r="F50" s="40"/>
-      <c r="G50" s="40"/>
-      <c r="H50" s="40"/>
-      <c r="I50" s="40"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="38"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="40"/>
-      <c r="B51" s="43" t="s">
+      <c r="A51" s="38"/>
+      <c r="B51" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="C51" s="48">
+      <c r="C51" s="46">
         <v>0.23</v>
       </c>
-      <c r="D51" s="48">
+      <c r="D51" s="46">
         <v>0.15</v>
       </c>
-      <c r="E51" s="48">
+      <c r="E51" s="46">
         <v>0.3</v>
       </c>
-      <c r="F51" s="40"/>
-      <c r="G51" s="40"/>
-      <c r="H51" s="40"/>
-      <c r="I51" s="40"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="38"/>
+      <c r="H51" s="38"/>
+      <c r="I51" s="38"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="40"/>
-      <c r="B52" s="43" t="s">
+      <c r="A52" s="38"/>
+      <c r="B52" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="48">
+      <c r="C52" s="46">
         <v>2.17</v>
       </c>
-      <c r="D52" s="48">
+      <c r="D52" s="46">
         <v>1.27</v>
       </c>
-      <c r="E52" s="48">
+      <c r="E52" s="46">
         <v>3.71</v>
       </c>
-      <c r="F52" s="40"/>
-      <c r="G52" s="40"/>
-      <c r="H52" s="40"/>
-      <c r="I52" s="40"/>
+      <c r="F52" s="38"/>
+      <c r="G52" s="38"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="38"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="40"/>
-      <c r="B53" s="42"/>
-      <c r="C53" s="40"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="40"/>
-      <c r="F53" s="40"/>
-      <c r="G53" s="40"/>
-      <c r="H53" s="40"/>
-      <c r="I53" s="40"/>
+      <c r="A53" s="38"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
+      <c r="I53" s="38"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="40"/>
-      <c r="B54" s="42"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="40"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="40"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="40"/>
-      <c r="I54" s="40"/>
+      <c r="A54" s="38"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="38"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="38"/>
+      <c r="H54" s="38"/>
+      <c r="I54" s="38"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="40"/>
-      <c r="B55" s="42"/>
-      <c r="C55" s="40"/>
-      <c r="D55" s="40"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="40"/>
-      <c r="G55" s="40"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="40"/>
+      <c r="A55" s="38"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="38"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="38"/>
+      <c r="H55" s="38"/>
+      <c r="I55" s="38"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="41" t="s">
+      <c r="A56" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="B56" s="42"/>
-      <c r="C56" s="40"/>
-      <c r="D56" s="40"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="40"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="38"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="38"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="40"/>
-      <c r="B57" s="42"/>
-      <c r="C57" s="44" t="s">
+      <c r="A57" s="38"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D57" s="44" t="s">
+      <c r="D57" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E57" s="44" t="s">
+      <c r="E57" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="F57" s="40"/>
-      <c r="G57" s="40"/>
-      <c r="H57" s="40"/>
-      <c r="I57" s="40"/>
+      <c r="F57" s="38"/>
+      <c r="G57" s="38"/>
+      <c r="H57" s="38"/>
+      <c r="I57" s="38"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="40"/>
-      <c r="B58" s="43" t="s">
+      <c r="A58" s="38"/>
+      <c r="B58" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C58" s="47">
+      <c r="C58" s="45">
         <v>0.7</v>
       </c>
-      <c r="D58" s="47">
+      <c r="D58" s="45">
         <v>0.5</v>
       </c>
-      <c r="E58" s="47">
+      <c r="E58" s="45">
         <v>0.9</v>
       </c>
-      <c r="F58" s="40"/>
-      <c r="G58" s="49"/>
-      <c r="H58" s="49"/>
-      <c r="I58" s="49"/>
+      <c r="F58" s="38"/>
+      <c r="G58" s="47"/>
+      <c r="H58" s="47"/>
+      <c r="I58" s="47"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="40"/>
-      <c r="B59" s="43" t="s">
+      <c r="A59" s="38"/>
+      <c r="B59" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C59" s="47">
+      <c r="C59" s="45">
         <v>0.9</v>
       </c>
-      <c r="D59" s="47">
+      <c r="D59" s="45">
         <v>0.82000000000000006</v>
       </c>
-      <c r="E59" s="47">
+      <c r="E59" s="45">
         <v>0.92999999999999994</v>
       </c>
-      <c r="F59" s="40"/>
-      <c r="G59" s="49"/>
-      <c r="H59" s="49"/>
-      <c r="I59" s="49"/>
+      <c r="F59" s="38"/>
+      <c r="G59" s="47"/>
+      <c r="H59" s="47"/>
+      <c r="I59" s="47"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="40"/>
-      <c r="B60" s="43" t="s">
+      <c r="A60" s="38"/>
+      <c r="B60" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="C60" s="47">
+      <c r="C60" s="45">
         <v>0.72499999999999998</v>
       </c>
-      <c r="D60" s="47">
+      <c r="D60" s="45">
         <v>0.65</v>
       </c>
-      <c r="E60" s="47">
+      <c r="E60" s="45">
         <v>0.8</v>
       </c>
-      <c r="F60" s="40"/>
-      <c r="G60" s="49"/>
-      <c r="H60" s="49"/>
-      <c r="I60" s="49"/>
+      <c r="F60" s="38"/>
+      <c r="G60" s="47"/>
+      <c r="H60" s="47"/>
+      <c r="I60" s="47"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="40"/>
-      <c r="B61" s="43" t="s">
+      <c r="A61" s="38"/>
+      <c r="B61" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="C61" s="47">
+      <c r="C61" s="45">
         <v>0.95</v>
       </c>
-      <c r="D61" s="47">
+      <c r="D61" s="45">
         <v>0.8</v>
       </c>
-      <c r="E61" s="47">
+      <c r="E61" s="45">
         <v>0.97499999999999998</v>
       </c>
-      <c r="F61" s="40"/>
-      <c r="G61" s="49"/>
-      <c r="H61" s="49"/>
-      <c r="I61" s="49"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="47"/>
+      <c r="H61" s="47"/>
+      <c r="I61" s="47"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="40"/>
-      <c r="B62" s="43" t="s">
+      <c r="A62" s="38"/>
+      <c r="B62" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="C62" s="47">
+      <c r="C62" s="45">
         <v>0.58000000000000007</v>
       </c>
-      <c r="D62" s="47">
+      <c r="D62" s="45">
         <v>0.47</v>
       </c>
-      <c r="E62" s="47">
+      <c r="E62" s="45">
         <v>0.66999999999999993</v>
       </c>
-      <c r="F62" s="40"/>
-      <c r="G62" s="49"/>
-      <c r="H62" s="49"/>
-      <c r="I62" s="49"/>
+      <c r="F62" s="38"/>
+      <c r="G62" s="47"/>
+      <c r="H62" s="47"/>
+      <c r="I62" s="47"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="40"/>
-      <c r="B63" s="43" t="s">
+      <c r="A63" s="38"/>
+      <c r="B63" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="C63" s="47">
+      <c r="C63" s="45">
         <v>0.54</v>
       </c>
-      <c r="D63" s="47">
+      <c r="D63" s="45">
         <v>0.32999999999999996</v>
       </c>
-      <c r="E63" s="47">
+      <c r="E63" s="45">
         <v>0.67999999999999994</v>
       </c>
-      <c r="F63" s="40"/>
-      <c r="G63" s="49"/>
-      <c r="H63" s="49"/>
-      <c r="I63" s="49"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="47"/>
+      <c r="H63" s="47"/>
+      <c r="I63" s="47"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="40"/>
-      <c r="B64" s="43" t="s">
+      <c r="A64" s="38"/>
+      <c r="B64" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="C64" s="47">
+      <c r="C64" s="45">
         <v>0</v>
       </c>
-      <c r="D64" s="47">
+      <c r="D64" s="45">
         <v>0</v>
       </c>
-      <c r="E64" s="47">
+      <c r="E64" s="45">
         <v>0.67999999999999994</v>
       </c>
-      <c r="F64" s="40"/>
-      <c r="G64" s="49"/>
-      <c r="H64" s="49"/>
-      <c r="I64" s="49"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="47"/>
+      <c r="H64" s="47"/>
+      <c r="I64" s="47"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="40"/>
-      <c r="B65" s="43" t="s">
+      <c r="A65" s="38"/>
+      <c r="B65" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="C65" s="47">
+      <c r="C65" s="45">
         <v>2.65</v>
       </c>
-      <c r="D65" s="47">
+      <c r="D65" s="45">
         <v>1.35</v>
       </c>
-      <c r="E65" s="47">
+      <c r="E65" s="45">
         <v>5.19</v>
       </c>
-      <c r="F65" s="40"/>
-      <c r="G65" s="49"/>
-      <c r="H65" s="49"/>
-      <c r="I65" s="49"/>
+      <c r="F65" s="38"/>
+      <c r="G65" s="47"/>
+      <c r="H65" s="47"/>
+      <c r="I65" s="47"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="40"/>
-      <c r="B66" s="42"/>
-      <c r="C66" s="40"/>
-      <c r="D66" s="40"/>
-      <c r="E66" s="40"/>
-      <c r="F66" s="40"/>
-      <c r="G66" s="40"/>
-      <c r="H66" s="40"/>
-      <c r="I66" s="40"/>
+      <c r="A66" s="38"/>
+      <c r="B66" s="40"/>
+      <c r="C66" s="38"/>
+      <c r="D66" s="38"/>
+      <c r="E66" s="38"/>
+      <c r="F66" s="38"/>
+      <c r="G66" s="38"/>
+      <c r="H66" s="38"/>
+      <c r="I66" s="38"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="40"/>
-      <c r="B67" s="42"/>
-      <c r="C67" s="40"/>
-      <c r="D67" s="40"/>
-      <c r="E67" s="40"/>
-      <c r="F67" s="40"/>
-      <c r="G67" s="40"/>
-      <c r="H67" s="40"/>
-      <c r="I67" s="40"/>
+      <c r="A67" s="38"/>
+      <c r="B67" s="40"/>
+      <c r="C67" s="38"/>
+      <c r="D67" s="38"/>
+      <c r="E67" s="38"/>
+      <c r="F67" s="38"/>
+      <c r="G67" s="38"/>
+      <c r="H67" s="38"/>
+      <c r="I67" s="38"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="40"/>
-      <c r="B68" s="42"/>
-      <c r="C68" s="40"/>
-      <c r="D68" s="40"/>
-      <c r="E68" s="40"/>
-      <c r="F68" s="40"/>
-      <c r="G68" s="40"/>
-      <c r="H68" s="40"/>
-      <c r="I68" s="40"/>
+      <c r="A68" s="38"/>
+      <c r="B68" s="40"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="38"/>
+      <c r="F68" s="38"/>
+      <c r="G68" s="38"/>
+      <c r="H68" s="38"/>
+      <c r="I68" s="38"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="41" t="s">
+      <c r="A69" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="B69" s="42"/>
-      <c r="C69" s="40"/>
-      <c r="D69" s="40"/>
-      <c r="E69" s="40"/>
-      <c r="F69" s="40"/>
-      <c r="G69" s="40"/>
-      <c r="H69" s="40"/>
-      <c r="I69" s="40"/>
+      <c r="B69" s="40"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="38"/>
+      <c r="H69" s="38"/>
+      <c r="I69" s="38"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="40"/>
-      <c r="B70" s="42"/>
-      <c r="C70" s="44" t="s">
+      <c r="A70" s="38"/>
+      <c r="B70" s="40"/>
+      <c r="C70" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D70" s="44" t="s">
+      <c r="D70" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E70" s="44" t="s">
+      <c r="E70" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="F70" s="40"/>
-      <c r="G70" s="40"/>
-      <c r="H70" s="40"/>
-      <c r="I70" s="40"/>
+      <c r="F70" s="38"/>
+      <c r="G70" s="38"/>
+      <c r="H70" s="38"/>
+      <c r="I70" s="38"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="40"/>
-      <c r="B71" s="43" t="s">
+      <c r="A71" s="38"/>
+      <c r="B71" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="C71" s="45">
+      <c r="C71" s="43">
         <v>0.14599999999999999</v>
       </c>
-      <c r="D71" s="45">
+      <c r="D71" s="43">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="E71" s="45">
+      <c r="E71" s="43">
         <v>0.20499999999999999</v>
       </c>
-      <c r="F71" s="40"/>
-      <c r="G71" s="40"/>
-      <c r="H71" s="40"/>
-      <c r="I71" s="40"/>
+      <c r="F71" s="38"/>
+      <c r="G71" s="38"/>
+      <c r="H71" s="38"/>
+      <c r="I71" s="38"/>
       <c r="J71" s="27"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="40"/>
-      <c r="B72" s="43" t="s">
+      <c r="A72" s="38"/>
+      <c r="B72" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="C72" s="45">
+      <c r="C72" s="43">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D72" s="45">
+      <c r="D72" s="43">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E72" s="45">
+      <c r="E72" s="43">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="F72" s="40"/>
-      <c r="G72" s="40"/>
-      <c r="H72" s="40"/>
-      <c r="I72" s="40"/>
+      <c r="F72" s="38"/>
+      <c r="G72" s="38"/>
+      <c r="H72" s="38"/>
+      <c r="I72" s="38"/>
       <c r="J72" s="27"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="40"/>
-      <c r="B73" s="43" t="s">
+      <c r="A73" s="38"/>
+      <c r="B73" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="C73" s="45">
+      <c r="C73" s="43">
         <v>0.02</v>
       </c>
-      <c r="D73" s="45">
+      <c r="D73" s="43">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="E73" s="45">
+      <c r="E73" s="43">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="F73" s="40"/>
-      <c r="G73" s="40"/>
-      <c r="H73" s="40"/>
-      <c r="I73" s="40"/>
+      <c r="F73" s="38"/>
+      <c r="G73" s="38"/>
+      <c r="H73" s="38"/>
+      <c r="I73" s="38"/>
       <c r="J73" s="27"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="40"/>
-      <c r="B74" s="43" t="s">
+      <c r="A74" s="38"/>
+      <c r="B74" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="C74" s="45">
+      <c r="C74" s="43">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D74" s="45">
+      <c r="D74" s="43">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E74" s="45">
+      <c r="E74" s="43">
         <v>9.4E-2</v>
       </c>
-      <c r="F74" s="40"/>
-      <c r="G74" s="40"/>
-      <c r="H74" s="40"/>
-      <c r="I74" s="40"/>
+      <c r="F74" s="38"/>
+      <c r="G74" s="38"/>
+      <c r="H74" s="38"/>
+      <c r="I74" s="38"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="40"/>
-      <c r="B75" s="43" t="s">
+      <c r="A75" s="38"/>
+      <c r="B75" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="C75" s="45">
+      <c r="C75" s="43">
         <v>0.26500000000000001</v>
       </c>
-      <c r="D75" s="45">
+      <c r="D75" s="43">
         <v>0.114</v>
       </c>
-      <c r="E75" s="45">
+      <c r="E75" s="43">
         <v>0.47399999999999998</v>
       </c>
-      <c r="F75" s="40"/>
-      <c r="G75" s="40"/>
-      <c r="H75" s="40"/>
-      <c r="I75" s="40"/>
+      <c r="F75" s="38"/>
+      <c r="G75" s="38"/>
+      <c r="H75" s="38"/>
+      <c r="I75" s="38"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="40"/>
-      <c r="B76" s="43" t="s">
+      <c r="A76" s="38"/>
+      <c r="B76" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="C76" s="45">
+      <c r="C76" s="43">
         <v>0.54700000000000004</v>
       </c>
-      <c r="D76" s="45">
+      <c r="D76" s="43">
         <v>0.38200000000000001</v>
       </c>
-      <c r="E76" s="45">
+      <c r="E76" s="43">
         <v>0.71499999999999997</v>
       </c>
-      <c r="F76" s="40"/>
-      <c r="G76" s="40"/>
-      <c r="H76" s="40"/>
-      <c r="I76" s="40"/>
+      <c r="F76" s="38"/>
+      <c r="G76" s="38"/>
+      <c r="H76" s="38"/>
+      <c r="I76" s="38"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="40"/>
-      <c r="B77" s="43" t="s">
+      <c r="A77" s="38"/>
+      <c r="B77" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="C77" s="45">
+      <c r="C77" s="43">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="D77" s="45">
+      <c r="D77" s="43">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="E77" s="45">
+      <c r="E77" s="43">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="F77" s="40"/>
-      <c r="G77" s="40"/>
-      <c r="H77" s="40"/>
-      <c r="I77" s="40"/>
+      <c r="F77" s="38"/>
+      <c r="G77" s="38"/>
+      <c r="H77" s="38"/>
+      <c r="I77" s="38"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C78" s="3"/>
@@ -3208,7 +3208,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3238,10 +3238,10 @@
       <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="31" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3503,7 +3503,7 @@
     </row>
     <row r="3" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -3537,7 +3537,7 @@
     </row>
     <row r="4" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -3593,7 +3593,7 @@
     </row>
     <row r="5" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -3627,7 +3627,7 @@
     </row>
     <row r="7" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -3661,7 +3661,7 @@
     </row>
     <row r="8" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -3717,7 +3717,7 @@
     </row>
     <row r="9" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -3751,7 +3751,7 @@
     </row>
     <row r="11" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -3785,7 +3785,7 @@
     </row>
     <row r="12" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -3841,7 +3841,7 @@
     </row>
     <row r="13" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -3888,7 +3888,7 @@
     </row>
     <row r="15" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -3922,7 +3922,7 @@
     </row>
     <row r="16" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -3978,7 +3978,7 @@
     </row>
     <row r="17" spans="2:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -4012,7 +4012,7 @@
     </row>
     <row r="19" spans="2:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -4046,7 +4046,7 @@
     </row>
     <row r="20" spans="2:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -4102,7 +4102,7 @@
     </row>
     <row r="21" spans="2:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -4136,7 +4136,7 @@
     </row>
     <row r="23" spans="2:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -4170,7 +4170,7 @@
     </row>
     <row r="24" spans="2:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -4226,7 +4226,7 @@
     </row>
     <row r="25" spans="2:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -4260,7 +4260,7 @@
     </row>
     <row r="27" spans="2:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -4294,7 +4294,7 @@
     </row>
     <row r="28" spans="2:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -4350,7 +4350,7 @@
     </row>
     <row r="29" spans="2:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -4517,7 +4517,7 @@
     </row>
     <row r="3" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -4551,7 +4551,7 @@
     </row>
     <row r="4" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -4591,7 +4591,7 @@
     </row>
     <row r="5" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -4625,7 +4625,7 @@
     </row>
     <row r="7" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -4659,7 +4659,7 @@
     </row>
     <row r="8" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -4695,7 +4695,7 @@
     </row>
     <row r="9" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -4729,7 +4729,7 @@
     </row>
     <row r="11" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -4763,7 +4763,7 @@
     </row>
     <row r="12" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -4805,7 +4805,7 @@
     </row>
     <row r="13" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -4839,7 +4839,7 @@
     </row>
     <row r="15" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -4873,7 +4873,7 @@
     </row>
     <row r="16" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -4909,7 +4909,7 @@
     </row>
     <row r="17" spans="2:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -4943,7 +4943,7 @@
     </row>
     <row r="19" spans="2:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -4977,7 +4977,7 @@
     </row>
     <row r="20" spans="2:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -5013,7 +5013,7 @@
     </row>
     <row r="21" spans="2:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -5047,7 +5047,7 @@
     </row>
     <row r="23" spans="2:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -5081,7 +5081,7 @@
     </row>
     <row r="24" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -5129,7 +5129,7 @@
     </row>
     <row r="25" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -5163,7 +5163,7 @@
     </row>
     <row r="27" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -5197,7 +5197,7 @@
     </row>
     <row r="28" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -5245,7 +5245,7 @@
     </row>
     <row r="29" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -5373,7 +5373,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C3" s="5"/>
@@ -5406,7 +5406,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C4" s="5"/>
@@ -5439,7 +5439,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C5" s="5"/>
@@ -5472,7 +5472,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C6" s="5"/>
@@ -5505,7 +5505,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C7" s="5"/>
@@ -5538,7 +5538,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C8" s="5"/>
@@ -5571,7 +5571,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C9" s="5"/>
@@ -5677,7 +5677,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C15" s="5"/>
@@ -5710,7 +5710,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C16" s="5"/>
@@ -5743,7 +5743,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C17" s="5"/>
@@ -5776,7 +5776,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C18" s="5"/>
@@ -5809,7 +5809,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C19" s="5"/>
@@ -5842,7 +5842,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C20" s="5"/>
@@ -5875,7 +5875,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C21" s="5"/>
@@ -5981,7 +5981,7 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C27" s="5"/>
@@ -6014,7 +6014,7 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C28" s="5"/>
@@ -6047,7 +6047,7 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C29" s="5"/>
@@ -6080,7 +6080,7 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C30" s="5"/>
@@ -6113,7 +6113,7 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C31" s="5"/>
@@ -6146,7 +6146,7 @@
     </row>
     <row r="32" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C32" s="5"/>
@@ -6179,7 +6179,7 @@
     </row>
     <row r="33" spans="2:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C33" s="5"/>
@@ -6725,185 +6725,185 @@
       <c r="Y21" s="8"/>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
-      <c r="O25" s="34"/>
-      <c r="P25" s="34"/>
-      <c r="Q25" s="34"/>
-      <c r="R25" s="34"/>
-      <c r="S25" s="34"/>
-      <c r="T25" s="34"/>
-      <c r="U25" s="34"/>
-      <c r="V25" s="34"/>
-      <c r="W25" s="34"/>
-      <c r="X25" s="34"/>
-      <c r="Y25" s="34"/>
-      <c r="Z25" s="34"/>
-      <c r="AA25" s="34"/>
-      <c r="AB25" s="34"/>
-      <c r="AC25" s="34"/>
-      <c r="AD25" s="34"/>
-      <c r="AE25" s="34"/>
-      <c r="AF25" s="34"/>
-      <c r="AG25" s="34"/>
-      <c r="AH25" s="34"/>
-      <c r="AI25" s="34"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="32"/>
+      <c r="W25" s="32"/>
+      <c r="X25" s="32"/>
+      <c r="Y25" s="32"/>
+      <c r="Z25" s="32"/>
+      <c r="AA25" s="32"/>
+      <c r="AB25" s="32"/>
+      <c r="AC25" s="32"/>
+      <c r="AD25" s="32"/>
+      <c r="AE25" s="32"/>
+      <c r="AF25" s="32"/>
+      <c r="AG25" s="32"/>
+      <c r="AH25" s="32"/>
+      <c r="AI25" s="32"/>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="36">
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="34">
         <v>2000</v>
       </c>
-      <c r="D26" s="36">
+      <c r="D26" s="34">
         <v>2001</v>
       </c>
-      <c r="E26" s="36">
+      <c r="E26" s="34">
         <v>2002</v>
       </c>
-      <c r="F26" s="36">
+      <c r="F26" s="34">
         <v>2003</v>
       </c>
-      <c r="G26" s="36">
+      <c r="G26" s="34">
         <v>2004</v>
       </c>
-      <c r="H26" s="36">
+      <c r="H26" s="34">
         <v>2005</v>
       </c>
-      <c r="I26" s="36">
+      <c r="I26" s="34">
         <v>2006</v>
       </c>
-      <c r="J26" s="36">
+      <c r="J26" s="34">
         <v>2007</v>
       </c>
-      <c r="K26" s="36">
+      <c r="K26" s="34">
         <v>2008</v>
       </c>
-      <c r="L26" s="36">
+      <c r="L26" s="34">
         <v>2009</v>
       </c>
-      <c r="M26" s="36">
+      <c r="M26" s="34">
         <v>2010</v>
       </c>
-      <c r="N26" s="36">
+      <c r="N26" s="34">
         <v>2011</v>
       </c>
-      <c r="O26" s="36">
+      <c r="O26" s="34">
         <v>2012</v>
       </c>
-      <c r="P26" s="36">
+      <c r="P26" s="34">
         <v>2013</v>
       </c>
-      <c r="Q26" s="36">
+      <c r="Q26" s="34">
         <v>2014</v>
       </c>
-      <c r="R26" s="36">
+      <c r="R26" s="34">
         <v>2015</v>
       </c>
-      <c r="S26" s="36">
+      <c r="S26" s="34">
         <v>2016</v>
       </c>
-      <c r="T26" s="36">
+      <c r="T26" s="34">
         <v>2017</v>
       </c>
-      <c r="U26" s="36">
+      <c r="U26" s="34">
         <v>2018</v>
       </c>
-      <c r="V26" s="36">
+      <c r="V26" s="34">
         <v>2019</v>
       </c>
-      <c r="W26" s="36">
+      <c r="W26" s="34">
         <v>2020</v>
       </c>
-      <c r="X26" s="36">
+      <c r="X26" s="34">
         <v>2021</v>
       </c>
-      <c r="Y26" s="36">
+      <c r="Y26" s="34">
         <v>2022</v>
       </c>
-      <c r="Z26" s="36">
+      <c r="Z26" s="34">
         <v>2023</v>
       </c>
-      <c r="AA26" s="36">
+      <c r="AA26" s="34">
         <v>2024</v>
       </c>
-      <c r="AB26" s="36">
+      <c r="AB26" s="34">
         <v>2025</v>
       </c>
-      <c r="AC26" s="36">
+      <c r="AC26" s="34">
         <v>2026</v>
       </c>
-      <c r="AD26" s="36">
+      <c r="AD26" s="34">
         <v>2027</v>
       </c>
-      <c r="AE26" s="36">
+      <c r="AE26" s="34">
         <v>2028</v>
       </c>
-      <c r="AF26" s="36">
+      <c r="AF26" s="34">
         <v>2029</v>
       </c>
-      <c r="AG26" s="36">
+      <c r="AG26" s="34">
         <v>2030</v>
       </c>
-      <c r="AH26" s="34"/>
-      <c r="AI26" s="36" t="s">
+      <c r="AH26" s="32"/>
+      <c r="AI26" s="34" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
-      <c r="B27" s="36" t="s">
+      <c r="A27" s="32"/>
+      <c r="B27" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="37"/>
-      <c r="P27" s="37"/>
-      <c r="Q27" s="37"/>
-      <c r="R27" s="37"/>
-      <c r="S27" s="37"/>
-      <c r="T27" s="37"/>
-      <c r="U27" s="37"/>
-      <c r="V27" s="37"/>
-      <c r="W27" s="37"/>
-      <c r="X27" s="37"/>
-      <c r="Y27" s="37"/>
-      <c r="Z27" s="37"/>
-      <c r="AA27" s="37"/>
-      <c r="AB27" s="37"/>
-      <c r="AC27" s="37"/>
-      <c r="AD27" s="37"/>
-      <c r="AE27" s="37"/>
-      <c r="AF27" s="37"/>
-      <c r="AG27" s="37"/>
-      <c r="AH27" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="AI27" s="37"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="35"/>
+      <c r="N27" s="35"/>
+      <c r="O27" s="35"/>
+      <c r="P27" s="35"/>
+      <c r="Q27" s="35"/>
+      <c r="R27" s="35"/>
+      <c r="S27" s="35"/>
+      <c r="T27" s="35"/>
+      <c r="U27" s="35"/>
+      <c r="V27" s="35"/>
+      <c r="W27" s="35"/>
+      <c r="X27" s="35"/>
+      <c r="Y27" s="35"/>
+      <c r="Z27" s="35"/>
+      <c r="AA27" s="35"/>
+      <c r="AB27" s="35"/>
+      <c r="AC27" s="35"/>
+      <c r="AD27" s="35"/>
+      <c r="AE27" s="35"/>
+      <c r="AF27" s="35"/>
+      <c r="AG27" s="35"/>
+      <c r="AH27" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI27" s="35"/>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -7157,7 +7157,7 @@
   <dimension ref="A1:Y54"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="S51" sqref="S51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7237,7 +7237,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C3" s="17"/>
@@ -7272,7 +7272,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C4" s="17"/>
@@ -7309,7 +7309,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C5" s="17"/>
@@ -7342,7 +7342,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C6" s="9"/>
@@ -7375,7 +7375,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C7" s="9"/>
@@ -7408,7 +7408,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C8" s="17"/>
@@ -7445,7 +7445,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C9" s="17"/>
@@ -7586,7 +7586,7 @@
       <c r="Y15" s="4"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="37" t="s">
         <v>110</v>
       </c>
     </row>
@@ -7781,7 +7781,7 @@
     </row>
     <row r="28" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C28" s="9"/>
@@ -7814,7 +7814,7 @@
     </row>
     <row r="29" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C29" s="9"/>
@@ -7847,7 +7847,7 @@
     </row>
     <row r="30" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C30" s="9"/>
@@ -7880,7 +7880,7 @@
     </row>
     <row r="31" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C31" s="9"/>
@@ -7913,7 +7913,7 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C32" s="9"/>
@@ -7946,7 +7946,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C33" s="9"/>
@@ -7979,7 +7979,7 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C34" s="9"/>
@@ -8192,7 +8192,7 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C46" s="21">
@@ -8245,7 +8245,7 @@
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C47" s="21"/>
@@ -8272,11 +8272,13 @@
       <c r="X47" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y47" s="8"/>
+      <c r="Y47" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C48" s="21">
@@ -8442,8 +8444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y78"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA25" sqref="AA25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8523,7 +8525,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C3" s="4"/>
@@ -8556,7 +8558,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C4" s="4"/>
@@ -8589,7 +8591,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C5" s="4"/>
@@ -8622,7 +8624,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C6" s="4"/>
@@ -8655,7 +8657,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C7" s="4"/>
@@ -8688,7 +8690,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C8" s="4"/>
@@ -8721,7 +8723,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C9" s="4"/>
@@ -8827,7 +8829,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C15" s="4"/>
@@ -8860,7 +8862,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C16" s="4"/>
@@ -8893,7 +8895,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C17" s="4"/>
@@ -8926,7 +8928,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C18" s="4"/>
@@ -8959,7 +8961,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C19" s="4"/>
@@ -8992,7 +8994,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C20" s="4"/>
@@ -9025,7 +9027,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C21" s="4"/>
@@ -9131,7 +9133,7 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C27" s="4"/>
@@ -9164,7 +9166,7 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C28" s="4"/>
@@ -9197,7 +9199,7 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C29" s="4"/>
@@ -9224,11 +9226,13 @@
       <c r="X29" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y29" s="4"/>
+      <c r="Y29" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C30" s="4"/>
@@ -9255,11 +9259,13 @@
       <c r="X30" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y30" s="4"/>
+      <c r="Y30" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C31" s="4"/>
@@ -9286,11 +9292,13 @@
       <c r="X31" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y31" s="4"/>
+      <c r="Y31" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C32" s="4"/>
@@ -9317,11 +9325,13 @@
       <c r="X32" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y32" s="4"/>
+      <c r="Y32" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C33" s="4"/>
@@ -9348,7 +9358,9 @@
       <c r="X33" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y33" s="4"/>
+      <c r="Y33" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -9425,7 +9437,7 @@
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C39" s="9"/>
@@ -9458,7 +9470,7 @@
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C40" s="9"/>
@@ -9491,7 +9503,7 @@
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C41" s="9"/>
@@ -9524,7 +9536,7 @@
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C42" s="9"/>
@@ -9551,11 +9563,13 @@
       <c r="X42" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y42" s="9"/>
+      <c r="Y42" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C43" s="9"/>
@@ -9582,11 +9596,13 @@
       <c r="X43" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y43" s="9"/>
+      <c r="Y43" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C44" s="9"/>
@@ -9619,7 +9635,7 @@
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C45" s="9"/>
@@ -9725,7 +9741,7 @@
     </row>
     <row r="51" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B51" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C51" s="9"/>
@@ -9758,7 +9774,7 @@
     </row>
     <row r="52" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B52" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C52" s="9"/>
@@ -9795,7 +9811,7 @@
     </row>
     <row r="53" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B53" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C53" s="9"/>
@@ -9828,7 +9844,7 @@
     </row>
     <row r="54" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B54" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C54" s="9"/>
@@ -9855,11 +9871,13 @@
       <c r="X54" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y54" s="9"/>
+      <c r="Y54" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B55" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C55" s="9"/>
@@ -9886,11 +9904,13 @@
       <c r="X55" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y55" s="9"/>
+      <c r="Y55" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B56" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C56" s="9"/>
@@ -9927,7 +9947,7 @@
     </row>
     <row r="57" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B57" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C57" s="9"/>
@@ -10037,7 +10057,7 @@
     </row>
     <row r="63" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B63" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C63" s="9"/>
@@ -10072,7 +10092,7 @@
     </row>
     <row r="64" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B64" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C64" s="9"/>
@@ -10099,11 +10119,13 @@
       <c r="X64" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y64" s="9"/>
+      <c r="Y64" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B65" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C65" s="9"/>
@@ -10130,11 +10152,13 @@
       <c r="X65" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y65" s="9"/>
+      <c r="Y65" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="66" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B66" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C66" s="9"/>
@@ -10161,11 +10185,13 @@
       <c r="X66" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y66" s="9"/>
+      <c r="Y66" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C67" s="9"/>
@@ -10192,11 +10218,13 @@
       <c r="X67" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y67" s="9"/>
+      <c r="Y67" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C68" s="9"/>
@@ -10223,11 +10251,13 @@
       <c r="X68" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y68" s="9"/>
+      <c r="Y68" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C69" s="9"/>
@@ -10254,7 +10284,9 @@
       <c r="X69" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y69" s="9"/>
+      <c r="Y69" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
@@ -10331,7 +10363,7 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C75" s="9"/>
@@ -10364,7 +10396,7 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C76" s="9"/>
@@ -10397,7 +10429,7 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C77" s="9"/>
@@ -10430,7 +10462,7 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C78" s="9"/>
@@ -10557,7 +10589,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C3" s="4"/>
@@ -10590,7 +10622,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C4" s="4"/>
@@ -10623,7 +10655,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C5" s="4"/>
@@ -10656,7 +10688,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C6" s="4"/>
@@ -10689,7 +10721,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C7" s="4"/>
@@ -10722,7 +10754,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C8" s="4"/>
@@ -10755,7 +10787,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C9" s="4"/>
@@ -10861,7 +10893,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
+        <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
       <c r="C15" s="9"/>
@@ -10894,7 +10926,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
+        <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
       <c r="C16" s="9"/>
@@ -10927,7 +10959,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
+        <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
       <c r="C17" s="9"/>
@@ -10960,7 +10992,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
+        <f>Populations!$C$6</f>
         <v>Males 0-14</v>
       </c>
       <c r="C18" s="9"/>
@@ -10993,7 +11025,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
+        <f>Populations!$C$7</f>
         <v>Females 0-14</v>
       </c>
       <c r="C19" s="9"/>
@@ -11026,7 +11058,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
+        <f>Populations!$C$8</f>
         <v>Males 15+</v>
       </c>
       <c r="C20" s="9"/>
@@ -11059,7 +11091,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="str">
-        <f>'Populations &amp; programs'!$C$9</f>
+        <f>Populations!$C$9</f>
         <v>Females 15+</v>
       </c>
       <c r="C21" s="9"/>

</xml_diff>

<commit_message>
factor not working because stupid lists
</commit_message>
<xml_diff>
--- a/optima/test7pops.xlsx
+++ b/optima/test7pops.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="19410" windowHeight="10950" tabRatio="901" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="19410" windowHeight="10950" tabRatio="901" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -811,7 +811,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -926,6 +926,15 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="67" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="168">
@@ -3219,7 +3228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -6236,8 +6245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6682,59 +6691,59 @@
       <c r="B21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="8">
-        <v>0.11</v>
-      </c>
-      <c r="D21" s="8">
-        <v>0.13</v>
-      </c>
-      <c r="E21" s="8">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F21" s="8">
-        <v>0.16</v>
-      </c>
-      <c r="G21" s="8">
-        <v>0.17</v>
-      </c>
-      <c r="H21" s="8">
-        <v>0.18</v>
-      </c>
-      <c r="I21" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="J21" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="K21" s="8">
-        <v>0.21</v>
-      </c>
-      <c r="L21" s="8">
-        <v>0.22</v>
-      </c>
-      <c r="M21" s="8">
-        <v>0.22</v>
-      </c>
-      <c r="N21" s="8">
-        <v>0.23</v>
-      </c>
-      <c r="O21" s="8">
-        <v>0.23</v>
-      </c>
-      <c r="P21" s="8">
-        <v>0.23</v>
-      </c>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
-      <c r="V21" s="8"/>
-      <c r="W21" s="8"/>
-      <c r="X21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y21" s="8"/>
+      <c r="C21" s="52">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="D21" s="52">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="E21" s="52">
+        <v>1.4E-3</v>
+      </c>
+      <c r="F21" s="52">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="G21" s="52">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="H21" s="52">
+        <v>1.8E-3</v>
+      </c>
+      <c r="I21" s="52">
+        <v>1.9E-3</v>
+      </c>
+      <c r="J21" s="52">
+        <v>2E-3</v>
+      </c>
+      <c r="K21" s="52">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="L21" s="52">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="M21" s="52">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="N21" s="52">
+        <v>2.3E-3</v>
+      </c>
+      <c r="O21" s="52">
+        <v>2.3E-3</v>
+      </c>
+      <c r="P21" s="52">
+        <v>2.3E-3</v>
+      </c>
+      <c r="Q21" s="52"/>
+      <c r="R21" s="52"/>
+      <c r="S21" s="52"/>
+      <c r="T21" s="52"/>
+      <c r="U21" s="52"/>
+      <c r="V21" s="52"/>
+      <c r="W21" s="52"/>
+      <c r="X21" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y21" s="50"/>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
@@ -9683,7 +9692,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C50" s="3">
         <v>2000</v>
       </c>
@@ -9751,7 +9760,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -9784,7 +9793,7 @@
       </c>
       <c r="Y51" s="9"/>
     </row>
-    <row r="52" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -9821,7 +9830,7 @@
       </c>
       <c r="Y52" s="9"/>
     </row>
-    <row r="53" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -9854,7 +9863,7 @@
       </c>
       <c r="Y53" s="9"/>
     </row>
-    <row r="54" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>
@@ -9887,7 +9896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>F 0-14</v>
@@ -9920,7 +9929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>M 15+</v>
@@ -9957,7 +9966,7 @@
       </c>
       <c r="Y56" s="9"/>
     </row>
-    <row r="57" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>F 15+</v>
@@ -9994,12 +10003,12 @@
       </c>
       <c r="Y57" s="9"/>
     </row>
-    <row r="61" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C62" s="3">
         <v>2000</v>
       </c>
@@ -10067,7 +10076,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -10102,7 +10111,7 @@
       </c>
       <c r="Y63" s="9"/>
     </row>
-    <row r="64" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -10135,7 +10144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -10168,7 +10177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>M 0-14</v>

</xml_diff>